<commit_message>
Test d'intégration et MAJ
Création d'un main servant au test d'intégration (sur MSP430G2553). Pas tout à fait fonctionnel... L'intégration du servomoteur n'est pas au point.
Comporte :
IR_sensor, movement, servomotor, UART.

Dernière chose principale à effectuer :
Communication SPI...

Ce module d'intégration reçoit d'une console des caractères interragissant sur le robot. Le pilotage du robot fonctionne jusqu'ici très bien.
</commit_message>
<xml_diff>
--- a/Documents/Prévision valeurs IR sensor.xlsx
+++ b/Documents/Prévision valeurs IR sensor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="21840" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -13,10 +13,6 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -302,11 +298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107923136"/>
-        <c:axId val="107922560"/>
+        <c:axId val="88053376"/>
+        <c:axId val="88053952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107923136"/>
+        <c:axId val="88053376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -316,12 +312,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107922560"/>
+        <c:crossAx val="88053952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107922560"/>
+        <c:axId val="88053952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -332,7 +328,357 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107923136"/>
+        <c:crossAx val="88053376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.42737860892388452"/>
+                  <c:y val="-4.0922645086030829E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$L$3:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$M$3:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>660</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="91362368"/>
+        <c:axId val="91361792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="91362368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91361792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="91361792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91362368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.087729658792651E-2"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.57216338582677162"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.38356014873140859"/>
+                  <c:y val="-0.18140419947506561"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$M$3:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>660</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$L$3:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="87316096"/>
+        <c:axId val="87315520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="87316096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87315520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="87315520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87316096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -381,6 +727,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -676,15 +1082,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B31"/>
+  <dimension ref="A2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -693,25 +1099,37 @@
         <v>1141.0540000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B31" si="0">-3.9346*A3 + 1180.4</f>
+        <f>-3.9346*A3 + 1180.4</f>
         <v>1101.7080000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>60</v>
+      </c>
+      <c r="M3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B3:B31" si="0">-3.9346*A4 + 1180.4</f>
         <v>1062.3620000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>30</v>
+      </c>
+      <c r="M4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40</v>
       </c>
@@ -719,8 +1137,14 @@
         <f t="shared" si="0"/>
         <v>1023.0160000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>25</v>
+      </c>
+      <c r="M5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -728,8 +1152,14 @@
         <f t="shared" si="0"/>
         <v>983.67000000000007</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>20</v>
+      </c>
+      <c r="M6">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60</v>
       </c>
@@ -737,8 +1167,14 @@
         <f t="shared" si="0"/>
         <v>944.32400000000007</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>15</v>
+      </c>
+      <c r="M7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>70</v>
       </c>
@@ -746,8 +1182,14 @@
         <f t="shared" si="0"/>
         <v>904.97800000000007</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>10</v>
+      </c>
+      <c r="M8">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80</v>
       </c>
@@ -755,8 +1197,14 @@
         <f t="shared" si="0"/>
         <v>865.63200000000006</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90</v>
       </c>
@@ -764,8 +1212,14 @@
         <f t="shared" si="0"/>
         <v>826.28600000000006</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100</v>
       </c>
@@ -774,7 +1228,7 @@
         <v>786.94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>110</v>
       </c>
@@ -783,7 +1237,7 @@
         <v>747.59400000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>120</v>
       </c>
@@ -792,7 +1246,7 @@
         <v>708.24800000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>130</v>
       </c>
@@ -801,7 +1255,7 @@
         <v>668.90200000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>140</v>
       </c>
@@ -810,7 +1264,7 @@
         <v>629.55600000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Maj code + rapport
</commit_message>
<xml_diff>
--- a/Documents/Prévision valeurs IR sensor.xlsx
+++ b/Documents/Prévision valeurs IR sensor.xlsx
@@ -298,11 +298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="88053376"/>
-        <c:axId val="88053952"/>
+        <c:axId val="90232448"/>
+        <c:axId val="90233024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88053376"/>
+        <c:axId val="90232448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -312,12 +312,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88053952"/>
+        <c:crossAx val="90233024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88053952"/>
+        <c:axId val="90233024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -328,7 +328,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88053376"/>
+        <c:crossAx val="90232448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -468,11 +468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91362368"/>
-        <c:axId val="91361792"/>
+        <c:axId val="114106368"/>
+        <c:axId val="114106944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91362368"/>
+        <c:axId val="114106368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,12 +482,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91361792"/>
+        <c:crossAx val="114106944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91361792"/>
+        <c:axId val="114106944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -498,7 +498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91362368"/>
+        <c:crossAx val="114106368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -572,6 +572,24 @@
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Feuil1!$M$3:$M$10</c:f>
@@ -648,11 +666,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87316096"/>
-        <c:axId val="87315520"/>
+        <c:axId val="114108672"/>
+        <c:axId val="114109248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87316096"/>
+        <c:axId val="114108672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,12 +680,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87315520"/>
+        <c:crossAx val="114109248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87315520"/>
+        <c:axId val="114109248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87316096"/>
+        <c:crossAx val="114108672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1085,7 +1103,7 @@
   <dimension ref="A2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1137,7 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B3:B31" si="0">-3.9346*A4 + 1180.4</f>
+        <f t="shared" ref="B4:B31" si="0">-3.9346*A4 + 1180.4</f>
         <v>1062.3620000000001</v>
       </c>
       <c r="L4">

</xml_diff>